<commit_message>
dùng specification hay cho createNative khi truy vấn, dùng Tika để check content type của file
</commit_message>
<xml_diff>
--- a/iam-service/src/main/resources/templates/users_template.xlsx
+++ b/iam-service/src/main/resources/templates/users_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\evotek\enterprise-platform\iam-service\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41FC763-C981-43E6-B17D-F4ADAB748D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937E17F9-9B9A-447F-9D9A-18941B0632A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,11 +22,11 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={02BB64DD-B776-4551-82A9-F1150065E6EC}</author>
+    <author>tc={D0C3DF10-E891-42F9-8ED8-11F1C27140EF}</author>
     <author>tc={5EC12291-D850-4546-B9D4-005B53FC7EFA}</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{02BB64DD-B776-4551-82A9-F1150065E6EC}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D0C3DF10-E891-42F9-8ED8-11F1C27140EF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -118,26 +118,26 @@
     <t>${user.province}</t>
   </si>
   <si>
+    <t>${user.birthday ? dateFormat.format(user.birthday) : ''}</t>
+  </si>
+  <si>
+    <t>${user.yearsOfEx ? user.yearsOfEx : 0}</t>
+  </si>
+  <si>
+    <t>${user.locked ? 'Yes' : 'No'}</t>
+  </si>
+  <si>
+    <t>${user.deleted ? 'Yes' : 'No'}</t>
+  </si>
+  <si>
     <t>${rowIndex + 1}</t>
-  </si>
-  <si>
-    <t>${user.birthday ? dateFormat.format(user.birthday) : ''}</t>
-  </si>
-  <si>
-    <t>${user.yearsOfEx ? user.yearsOfEx : 0}</t>
-  </si>
-  <si>
-    <t>${user.locked ? 'Yes' : 'No'}</t>
-  </si>
-  <si>
-    <t>${user.deleted ? 'Yes' : 'No'}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -161,12 +161,6 @@
       <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -563,7 +557,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A1" dT="2025-11-13T09:08:24.37" personId="{32AE8309-BA7F-4D33-B70E-75E2AB2592FB}" id="{02BB64DD-B776-4551-82A9-F1150065E6EC}">
+  <threadedComment ref="A1" dT="2025-11-14T03:52:32.15" personId="{32AE8309-BA7F-4D33-B70E-75E2AB2592FB}" id="{D0C3DF10-E891-42F9-8ED8-11F1C27140EF}">
     <text>jx:area(lastCell="N2")</text>
   </threadedComment>
   <threadedComment ref="A2" dT="2025-11-13T08:21:11.21" personId="{32AE8309-BA7F-4D33-B70E-75E2AB2592FB}" id="{5EC12291-D850-4546-B9D4-005B53FC7EFA}">
@@ -644,7 +638,7 @@
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
@@ -659,7 +653,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>18</v>
@@ -677,13 +671,13 @@
         <v>22</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>